<commit_message>
model importation via csv términé
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Contenu</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>A faire</t>
+  </si>
+  <si>
+    <t>Réinitialisation donnée</t>
+  </si>
+  <si>
+    <t>Modele importation csv</t>
+  </si>
+  <si>
+    <t>Faire marché le projet</t>
+  </si>
+  <si>
+    <t>Comprendre le projet</t>
   </si>
 </sst>
 </file>
@@ -68,7 +80,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,6 +90,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -109,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -117,7 +141,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E4"/>
+  <dimension ref="A3:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,12 +457,51 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="5">
         <v>0.35833333333333334</v>
       </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
page list des devis terminé
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Contenu</t>
   </si>
@@ -70,6 +70,30 @@
   </si>
   <si>
     <t>Créer un controller pour gérer les requettes du login</t>
+  </si>
+  <si>
+    <t>Choisir un fournisseur</t>
+  </si>
+  <si>
+    <t>name, supplier_name</t>
+  </si>
+  <si>
+    <t>Créer une page pour choisir le fournisseur</t>
+  </si>
+  <si>
+    <t>Créer un controller pour gérer les requettes sur fournisseur</t>
+  </si>
+  <si>
+    <t>Listé les demandes de devis</t>
+  </si>
+  <si>
+    <t>Créer une page pour lister les demandes de devis</t>
+  </si>
+  <si>
+    <t>information à afficher(name, customer_name, transaction_date, order_type, company, total_quantity , base total)</t>
+  </si>
+  <si>
+    <t>49min</t>
   </si>
 </sst>
 </file>
@@ -154,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -164,10 +188,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,25 +496,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E13"/>
+  <dimension ref="A3:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -484,10 +531,10 @@
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="5">
+      <c r="E4" s="12">
         <v>0.35833333333333334</v>
       </c>
     </row>
@@ -495,83 +542,171 @@
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="12"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="13"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="13"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="11"/>
+      <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="11"/>
+      <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="6"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="13"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout page modification prix
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Contenu</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>49min</t>
+  </si>
+  <si>
+    <t>16h58-23h29</t>
   </si>
 </sst>
 </file>
@@ -204,17 +207,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +510,7 @@
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="54.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44" style="7" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -534,7 +537,7 @@
       <c r="B4" s="8"/>
       <c r="C4" s="6"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>0.35833333333333334</v>
       </c>
     </row>
@@ -545,7 +548,7 @@
       <c r="B5" s="8"/>
       <c r="C5" s="6"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="12"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -554,7 +557,7 @@
       <c r="B6" s="8"/>
       <c r="C6" s="6"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -563,7 +566,7 @@
       <c r="B7" s="8"/>
       <c r="C7" s="6"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="13"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -572,10 +575,10 @@
       <c r="B8" s="8"/>
       <c r="C8" s="6"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -585,19 +588,19 @@
         <v>12</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="13"/>
+      <c r="E11" s="12"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
@@ -605,19 +608,19 @@
         <v>15</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="13"/>
+      <c r="E12" s="12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -627,19 +630,19 @@
         <v>18</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="13"/>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="8" t="s">
         <v>19</v>
       </c>
@@ -647,19 +650,19 @@
         <v>15</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -669,19 +672,21 @@
         <v>18</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="13"/>
+      <c r="E18" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="13"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="8" t="s">
         <v>22</v>
       </c>
@@ -689,18 +694,18 @@
         <v>23</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="13"/>
+      <c r="E21" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>